<commit_message>
BOM: Alternatives TSV7722IQ2T, MAX942EUA+ added
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">BOM Version: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrokey TRNG RS232 - Tartaros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19. Aug. 2022</t>
+  </si>
   <si>
     <t xml:space="preserve">RD</t>
   </si>
@@ -43,6 +52,9 @@
     <t xml:space="preserve">URL</t>
   </si>
   <si>
+    <t xml:space="preserve">Alternative</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;  C1, C2</t>
   </si>
   <si>
@@ -196,6 +208,9 @@
     <t xml:space="preserve">https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART</t>
   </si>
   <si>
+    <t xml:space="preserve">TSV7722IQ2T</t>
+  </si>
+  <si>
     <t xml:space="preserve">    U5</t>
   </si>
   <si>
@@ -206,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX942EUA+</t>
   </si>
   <si>
     <t xml:space="preserve">    U6</t>
@@ -242,14 +260,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -267,8 +287,8 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -278,6 +298,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,12 +343,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,105 +377,92 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="84.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,10 +473,10 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,10 +487,10 @@
         <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,84 +501,84 @@
         <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1050170001</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1050170001</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,10 +589,10 @@
         <v>42</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,154 +603,188 @@
         <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>71</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://www.digikey.de/en/products/detail/GRM1885C1H221JA01D/490-1435-1-ND/587673?curr=usd"/>
-    <hyperlink ref="G8" r:id="rId2" display="https://www.digikey.de/de/products/detail/molex/1050170001/2350832"/>
-    <hyperlink ref="G9" r:id="rId3" display="https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087"/>
-    <hyperlink ref="G14" r:id="rId4" display="https://www.mouser.de/ProductDetail/Microchip-Technology-Atmel/ATMEGA16U2-MU?qs=JV7lzlMm3yIZlyznMyuPNA%3D%3D"/>
-    <hyperlink ref="G15" r:id="rId5" display="https://de.farnell.com/webapp/wcs/stores/servlet/ProductDisplay?catalogId=15001&amp;CMP=GRHB-OCTOPART&amp;productSeoURL=onsemi&amp;partNumber=2531589&amp;storeId=10161&amp;langId=-3&amp;krypto=MtGyFT4IPHKjHb1ikIgAFcglmNOWTSpVlwbwEsHlCUWCbbk%2B8Zb%2Fyr33uVmmwcPjkcZwcesuJIf39NMnhqGhiw%3D%3D"/>
-    <hyperlink ref="G16" r:id="rId6" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART"/>
-    <hyperlink ref="G17" r:id="rId7" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
-    <hyperlink ref="G18" r:id="rId8" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
-    <hyperlink ref="G19" r:id="rId9" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
+    <hyperlink ref="G4" r:id="rId1" display="https://www.digikey.de/en/products/detail/GRM1885C1H221JA01D/490-1435-1-ND/587673?curr=usd"/>
+    <hyperlink ref="G10" r:id="rId2" display="https://www.digikey.de/de/products/detail/molex/1050170001/2350832"/>
+    <hyperlink ref="G11" r:id="rId3" display="https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087"/>
+    <hyperlink ref="G16" r:id="rId4" display="https://www.mouser.de/ProductDetail/Microchip-Technology-Atmel/ATMEGA16U2-MU?qs=JV7lzlMm3yIZlyznMyuPNA%3D%3D"/>
+    <hyperlink ref="G17" r:id="rId5" display="https://de.farnell.com/webapp/wcs/stores/servlet/ProductDisplay?catalogId=15001&amp;CMP=GRHB-OCTOPART&amp;productSeoURL=onsemi&amp;partNumber=2531589&amp;storeId=10161&amp;langId=-3&amp;krypto=MtGyFT4IPHKjHb1ikIgAFcglmNOWTSpVlwbwEsHlCUWCbbk%2B8Zb%2Fyr33uVmmwcPjkcZwcesuJIf39NMnhqGhiw%3D%3D"/>
+    <hyperlink ref="G18" r:id="rId6" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART"/>
+    <hyperlink ref="G19" r:id="rId7" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
+    <hyperlink ref="G20" r:id="rId8" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
+    <hyperlink ref="G21" r:id="rId9" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed alternatives from BOM
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t xml:space="preserve">BOM Version: 2</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">URL</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;  C1, C2</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t xml:space="preserve">https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART</t>
   </si>
   <si>
-    <t xml:space="preserve">TSV7722IQ2T</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U5</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX942EUA+</t>
   </si>
   <si>
     <t xml:space="preserve">    U6</t>
@@ -377,18 +368,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="84.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,6 +393,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -424,42 +417,40 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -467,13 +458,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2</v>
@@ -481,13 +472,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4</v>
@@ -495,13 +486,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>3</v>
@@ -509,13 +500,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -523,59 +514,59 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1050170001</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -583,13 +574,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="C13" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>7</v>
@@ -597,13 +588,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -611,13 +602,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -625,146 +616,140 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="F18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="F20" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM: Added TC75W57FU as alternative
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t xml:space="preserve">BOM Version: 2</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">URL</t>
   </si>
   <si>
+    <t xml:space="preserve">Alternative</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;  C1, C2</t>
   </si>
   <si>
@@ -215,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC75W57FU</t>
   </si>
   <si>
     <t xml:space="preserve">    U6</t>
@@ -370,11 +376,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.8"/>
@@ -417,40 +423,43 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -458,13 +467,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2</v>
@@ -472,13 +481,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4</v>
@@ -486,13 +495,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>3</v>
@@ -500,13 +509,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -514,59 +523,59 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1050170001</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -574,13 +583,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>7</v>
@@ -588,13 +597,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -602,13 +611,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -616,140 +625,143 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM don't place J3, alternative for U2, U3
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
-  <si>
-    <t xml:space="preserve">BOM Version: 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+  <si>
+    <t xml:space="preserve">BOM Version: 3</t>
   </si>
   <si>
     <t xml:space="preserve">Nitrokey TRNG RS232 - Tartaros</t>
   </si>
   <si>
-    <t xml:space="preserve">24. Nov. 2022</t>
+    <t xml:space="preserve">26.2.2025</t>
   </si>
   <si>
     <t xml:space="preserve">RD</t>
@@ -121,7 +121,23 @@
     <t xml:space="preserve">https://www.digikey.de/de/products/detail/molex/1050170001/2350832</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;  J1, J3</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">J1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SFH11-PBPC-D05-ST-BK</t>
@@ -136,6 +152,28 @@
     <t xml:space="preserve">https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">J3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DNP</t>
+  </si>
+  <si>
     <t xml:space="preserve">&gt;  R1, R2</t>
   </si>
   <si>
@@ -163,7 +201,7 @@
     <t xml:space="preserve">27R 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">    U1</t>
+    <t xml:space="preserve">U1</t>
   </si>
   <si>
     <t xml:space="preserve">ATmega16U2-M</t>
@@ -190,7 +228,10 @@
     <t xml:space="preserve">onsemi</t>
   </si>
   <si>
-    <t xml:space="preserve">https://de.farnell.com/webapp/wcs/stores/servlet/ProductDisplay?catalogId=15001&amp;CMP=GRHB-OCTOPART&amp;productSeoURL=onsemi&amp;partNumber=2531589&amp;storeId=10161&amp;langId=-3&amp;krypto=MtGyFT4IPHKjHb1ikIgAFcglmNOWTSpVlwbwEsHlCUWCbbk%2B8Zb%2Fyr33uVmmwcPjkcZwcesuJIf39NMnhqGhiw%3D%3D</t>
+    <t xml:space="preserve">https://de.farnell.com/onsemi/mc74vhc1g66dft1g/analogschalter-1-kan-spst-no-ss/dp/2531589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.de/en/products/detail/nexperia-usa-inc/74AHC1G66GW-125/2814002</t>
   </si>
   <si>
     <t xml:space="preserve">    U4</t>
@@ -205,7 +246,7 @@
     <t xml:space="preserve">ST</t>
   </si>
   <si>
-    <t xml:space="preserve">https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART</t>
+    <t xml:space="preserve">https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662</t>
   </si>
   <si>
     <t xml:space="preserve">    U5</t>
@@ -261,7 +302,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -289,6 +330,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -340,20 +393,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,399 +434,525 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="84.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="104.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="73.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="AMJ1" s="1"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AMJ3" s="0"/>
+      <c r="AMJ3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>1050170001</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="0" t="n">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="0" t="n">
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="E19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="0" t="n">
+      <c r="F20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="E21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="E22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -769,12 +960,13 @@
     <hyperlink ref="G4" r:id="rId1" display="https://www.digikey.de/en/products/detail/GRM1885C1H221JA01D/490-1435-1-ND/587673?curr=usd"/>
     <hyperlink ref="G10" r:id="rId2" display="https://www.digikey.de/de/products/detail/molex/1050170001/2350832"/>
     <hyperlink ref="G11" r:id="rId3" display="https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087"/>
-    <hyperlink ref="G16" r:id="rId4" display="https://www.mouser.de/ProductDetail/Microchip-Technology-Atmel/ATMEGA16U2-MU?qs=JV7lzlMm3yIZlyznMyuPNA%3D%3D"/>
-    <hyperlink ref="G17" r:id="rId5" display="https://de.farnell.com/webapp/wcs/stores/servlet/ProductDisplay?catalogId=15001&amp;CMP=GRHB-OCTOPART&amp;productSeoURL=onsemi&amp;partNumber=2531589&amp;storeId=10161&amp;langId=-3&amp;krypto=MtGyFT4IPHKjHb1ikIgAFcglmNOWTSpVlwbwEsHlCUWCbbk%2B8Zb%2Fyr33uVmmwcPjkcZwcesuJIf39NMnhqGhiw%3D%3D"/>
-    <hyperlink ref="G18" r:id="rId6" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662?CMP=GRHB-OCTOPART"/>
-    <hyperlink ref="G19" r:id="rId7" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
-    <hyperlink ref="G20" r:id="rId8" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
-    <hyperlink ref="G21" r:id="rId9" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
+    <hyperlink ref="G17" r:id="rId4" display="https://www.mouser.de/ProductDetail/Microchip-Technology-Atmel/ATMEGA16U2-MU?qs=JV7lzlMm3yIZlyznMyuPNA%3D%3D"/>
+    <hyperlink ref="G18" r:id="rId5" display="https://de.farnell.com/onsemi/mc74vhc1g66dft1g/analogschalter-1-kan-spst-no-ss/dp/2531589"/>
+    <hyperlink ref="H18" r:id="rId6" display="https://www.digikey.de/en/products/detail/nexperia-usa-inc/74AHC1G66GW-125/2814002"/>
+    <hyperlink ref="G19" r:id="rId7" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662"/>
+    <hyperlink ref="G20" r:id="rId8" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
+    <hyperlink ref="G21" r:id="rId9" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
+    <hyperlink ref="G22" r:id="rId10" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
BOM v4: fix C4, C6 to 0603
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -20,17 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
-  <si>
-    <t xml:space="preserve">BOM Version: 3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
+  <si>
+    <t xml:space="preserve">BOM Version: 4</t>
   </si>
   <si>
     <t xml:space="preserve">Nitrokey TRNG RS232 - Tartaros</t>
   </si>
   <si>
-    <t xml:space="preserve">26.2.2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">RD</t>
   </si>
   <si>
@@ -121,23 +118,7 @@
     <t xml:space="preserve">https://www.digikey.de/de/products/detail/molex/1050170001/2350832</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">J1</t>
-    </r>
+    <t xml:space="preserve">    J1</t>
   </si>
   <si>
     <t xml:space="preserve">SFH11-PBPC-D05-ST-BK</t>
@@ -152,23 +133,7 @@
     <t xml:space="preserve">https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">J3</t>
-    </r>
+    <t xml:space="preserve">    J3</t>
   </si>
   <si>
     <t xml:space="preserve">DNP</t>
@@ -302,7 +267,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -330,18 +295,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -393,7 +346,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,11 +367,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,7 +497,7 @@
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,9 +505,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="104.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="73.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="73.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -569,70 +518,70 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
+      <c r="C1" s="3" t="n">
+        <v>45748</v>
       </c>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="AMJ3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -640,13 +589,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -654,13 +603,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>4</v>
@@ -668,13 +617,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>3</v>
@@ -682,13 +631,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -696,73 +645,72 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1050170001</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>2</v>
@@ -770,13 +718,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>7</v>
@@ -784,13 +732,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1</v>
@@ -798,13 +746,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>2</v>
@@ -813,146 +761,146 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM v5: U2, U3: Nexperia 74HCT1G66GW,125
</commit_message>
<xml_diff>
--- a/trng-serial-bom.xlsx
+++ b/trng-serial-bom.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
-  <si>
-    <t xml:space="preserve">BOM Version: 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">BOM Version: 5</t>
   </si>
   <si>
     <t xml:space="preserve">Nitrokey TRNG RS232 - Tartaros</t>
@@ -184,19 +184,16 @@
     <t xml:space="preserve">&gt;  U2, U3</t>
   </si>
   <si>
-    <t xml:space="preserve">MC74VHC1G66DFT1G</t>
+    <t xml:space="preserve">74HCT1G66GW,125</t>
   </si>
   <si>
     <t xml:space="preserve">Package_TO_SOT_SMD:SOT-353_SC-70-5</t>
   </si>
   <si>
-    <t xml:space="preserve">onsemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://de.farnell.com/onsemi/mc74vhc1g66dft1g/analogschalter-1-kan-spst-no-ss/dp/2531589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.de/en/products/detail/nexperia-usa-inc/74AHC1G66GW-125/2814002</t>
+    <t xml:space="preserve">Nexperia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.de/short/f9nwvdrf</t>
   </si>
   <si>
     <t xml:space="preserve">    U4</t>
@@ -519,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="n">
-        <v>45748</v>
+        <v>45926</v>
       </c>
       <c r="AMJ1" s="1"/>
     </row>
@@ -804,103 +801,101 @@
       <c r="G18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -909,12 +904,10 @@
     <hyperlink ref="G10" r:id="rId2" display="https://www.digikey.de/de/products/detail/molex/1050170001/2350832"/>
     <hyperlink ref="G11" r:id="rId3" display="https://www.digikey.de/de/products/detail/sullins-connector-solutions/SFH11-PBPC-D05-ST-BK/1990087"/>
     <hyperlink ref="G17" r:id="rId4" display="https://www.mouser.de/ProductDetail/Microchip-Technology-Atmel/ATMEGA16U2-MU?qs=JV7lzlMm3yIZlyznMyuPNA%3D%3D"/>
-    <hyperlink ref="G18" r:id="rId5" display="https://de.farnell.com/onsemi/mc74vhc1g66dft1g/analogschalter-1-kan-spst-no-ss/dp/2531589"/>
-    <hyperlink ref="H18" r:id="rId6" display="https://www.digikey.de/en/products/detail/nexperia-usa-inc/74AHC1G66GW-125/2814002"/>
-    <hyperlink ref="G19" r:id="rId7" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662"/>
-    <hyperlink ref="G20" r:id="rId8" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
-    <hyperlink ref="G21" r:id="rId9" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
-    <hyperlink ref="G22" r:id="rId10" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
+    <hyperlink ref="G19" r:id="rId5" display="https://de.farnell.com/stmicroelectronics/tsv912iq2t/op-verst-rker-8mhz-4-5v-us-dfn/dp/2762662"/>
+    <hyperlink ref="G20" r:id="rId6" display="https://www.digikey.de/en/products/detail/stmicroelectronics/TS3022IYST/8321879"/>
+    <hyperlink ref="G21" r:id="rId7" display="https://www.digikey.de/de/products/detail/texas-instruments/SN75C3221PWR/484694"/>
+    <hyperlink ref="G22" r:id="rId8" display="https://www.digikey.de/de/products/detail/abracon-llc/ABM8-16-000MHZ-B2-T/675329"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>